<commit_message>
new versions of the data
</commit_message>
<xml_diff>
--- a/static/data/PHM-EVD-contacts-2017-10-27.xlsx
+++ b/static/data/PHM-EVD-contacts-2017-10-27.xlsx
@@ -20,40 +20,40 @@
     <t>to</t>
   </si>
   <si>
+    <t>51883d</t>
+  </si>
+  <si>
+    <t>b4d8aa</t>
+  </si>
+  <si>
+    <t>39e9dc</t>
+  </si>
+  <si>
+    <t>185911</t>
+  </si>
+  <si>
+    <t>e4b0a2</t>
+  </si>
+  <si>
+    <t>601d2e</t>
+  </si>
+  <si>
+    <t>9aa197</t>
+  </si>
+  <si>
+    <t>e399b1</t>
+  </si>
+  <si>
+    <t>af0ac0</t>
+  </si>
+  <si>
     <t>947e40</t>
   </si>
   <si>
-    <t>1b6cc2</t>
-  </si>
-  <si>
-    <t>c61339</t>
+    <t>664549</t>
   </si>
   <si>
     <t>605322</t>
-  </si>
-  <si>
-    <t>d53618</t>
-  </si>
-  <si>
-    <t>e399b1</t>
-  </si>
-  <si>
-    <t>af0ac0</t>
-  </si>
-  <si>
-    <t>cca468</t>
-  </si>
-  <si>
-    <t>601d2e</t>
-  </si>
-  <si>
-    <t>e4b0a2</t>
-  </si>
-  <si>
-    <t>b8551b</t>
-  </si>
-  <si>
-    <t>3d8cf7</t>
   </si>
 </sst>
 </file>

</xml_diff>